<commit_message>
2019-10-15 19:19 agrgrega t=0 a pretrat y concatena todo en un mismo archivo
</commit_message>
<xml_diff>
--- a/resultados/aleatoriedad-inicio/aleatoriedad-elo-regular.xlsx
+++ b/resultados/aleatoriedad-inicio/aleatoriedad-elo-regular.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="230">
   <si>
     <t>Indicador</t>
   </si>
@@ -38,6 +38,9 @@
     <t>All</t>
   </si>
   <si>
+    <t>Frac. Fácil ELO p3 c3</t>
+  </si>
+  <si>
     <t>Frac. Fácil ELO p4 c3</t>
   </si>
   <si>
@@ -47,7 +50,7 @@
     <t>Frac. Fácil ELO p6 c3</t>
   </si>
   <si>
-    <t>Frac. Fácil ELO p7 c3</t>
+    <t>Frac. Fácil ELO p3 c4</t>
   </si>
   <si>
     <t>Frac. Fácil ELO p4 c4</t>
@@ -59,7 +62,7 @@
     <t>Frac. Fácil ELO p6 c4</t>
   </si>
   <si>
-    <t>Frac. Fácil ELO p7 c4</t>
+    <t>Frac. Fácil ELO p3 c5</t>
   </si>
   <si>
     <t>Frac. Fácil ELO p4 c5</t>
@@ -71,7 +74,19 @@
     <t>Frac. Fácil ELO p6 c5</t>
   </si>
   <si>
-    <t>Frac. Fácil ELO p7 c5</t>
+    <t>Frac. Fácil ELO p3 c6</t>
+  </si>
+  <si>
+    <t>Frac. Fácil ELO p4 c6</t>
+  </si>
+  <si>
+    <t>Frac. Fácil ELO p5 c6</t>
+  </si>
+  <si>
+    <t>Frac. Fácil ELO p6 c6</t>
+  </si>
+  <si>
+    <t>0.504 (N = 180)</t>
   </si>
   <si>
     <t>0.282 (N = 180)</t>
@@ -83,7 +98,7 @@
     <t>0.031 (N = 180)</t>
   </si>
   <si>
-    <t>0.005 (N = 180)</t>
+    <t>0.346 (N = 150)</t>
   </si>
   <si>
     <t>0.326 (N = 150)</t>
@@ -95,7 +110,7 @@
     <t>0.035 (N = 150)</t>
   </si>
   <si>
-    <t>0.0 (N = 150)</t>
+    <t>0.45 (N = 120)</t>
   </si>
   <si>
     <t>0.58 (N = 120)</t>
@@ -107,7 +122,19 @@
     <t>0.218 (N = 120)</t>
   </si>
   <si>
-    <t>0.05 (N = 120)</t>
+    <t>0.152 (N = 90)</t>
+  </si>
+  <si>
+    <t>0.238 (N = 90)</t>
+  </si>
+  <si>
+    <t>0.419 (N = 90)</t>
+  </si>
+  <si>
+    <t>0.597 (N = 90)</t>
+  </si>
+  <si>
+    <t>0.021 (N = 210)</t>
   </si>
   <si>
     <t>0.028 (N = 210)</t>
@@ -119,7 +146,7 @@
     <t>0.064 (N = 210)</t>
   </si>
   <si>
-    <t>0.065 (N = 210)</t>
+    <t>0.428 (N = 180)</t>
   </si>
   <si>
     <t>0.094 (N = 180)</t>
@@ -131,7 +158,7 @@
     <t>0.092 (N = 180)</t>
   </si>
   <si>
-    <t>0.072 (N = 180)</t>
+    <t>0.153 (N = 150)</t>
   </si>
   <si>
     <t>0.049 (N = 150)</t>
@@ -140,7 +167,19 @@
     <t>0.061 (N = 150)</t>
   </si>
   <si>
-    <t>0.012 (N = 150)</t>
+    <t>0.435 (N = 120)</t>
+  </si>
+  <si>
+    <t>0.103 (N = 120)</t>
+  </si>
+  <si>
+    <t>0.064 (N = 120)</t>
+  </si>
+  <si>
+    <t>0.006 (N = 120)</t>
+  </si>
+  <si>
+    <t>0.097 (N = 140)</t>
   </si>
   <si>
     <t>0.028 (N = 140)</t>
@@ -152,7 +191,7 @@
     <t>0.111 (N = 140)</t>
   </si>
   <si>
-    <t>0.113 (N = 140)</t>
+    <t>0.339 (N = 120)</t>
   </si>
   <si>
     <t>0.326 (N = 120)</t>
@@ -164,7 +203,7 @@
     <t>0.87 (N = 120)</t>
   </si>
   <si>
-    <t>0.671 (N = 120)</t>
+    <t>0.938 (N = 100)</t>
   </si>
   <si>
     <t>0.855 (N = 100)</t>
@@ -176,7 +215,19 @@
     <t>0.708 (N = 100)</t>
   </si>
   <si>
-    <t>0.745 (N = 100)</t>
+    <t>0.92 (N = 80)</t>
+  </si>
+  <si>
+    <t>0.791 (N = 80)</t>
+  </si>
+  <si>
+    <t>0.683 (N = 80)</t>
+  </si>
+  <si>
+    <t>0.702 (N = 80)</t>
+  </si>
+  <si>
+    <t>0.063 (N = 354)</t>
   </si>
   <si>
     <t>0.135 (N = 354)</t>
@@ -188,7 +239,7 @@
     <t>0.318 (N = 354)</t>
   </si>
   <si>
-    <t>0.864 (N = 354)</t>
+    <t>0.458 (N = 304)</t>
   </si>
   <si>
     <t>0.576 (N = 304)</t>
@@ -200,7 +251,7 @@
     <t>0.728 (N = 304)</t>
   </si>
   <si>
-    <t>0.758 (N = 304)</t>
+    <t>0.322 (N = 254)</t>
   </si>
   <si>
     <t>0.496 (N = 254)</t>
@@ -212,7 +263,19 @@
     <t>0.346 (N = 254)</t>
   </si>
   <si>
-    <t>0.669 (N = 254)</t>
+    <t>0.423 (N = 204)</t>
+  </si>
+  <si>
+    <t>0.357 (N = 204)</t>
+  </si>
+  <si>
+    <t>0.234 (N = 204)</t>
+  </si>
+  <si>
+    <t>0.083 (N = 204)</t>
+  </si>
+  <si>
+    <t>0.975 (N = 208)</t>
   </si>
   <si>
     <t>0.902 (N = 208)</t>
@@ -224,7 +287,7 @@
     <t>0.866 (N = 208)</t>
   </si>
   <si>
-    <t>0.524 (N = 208)</t>
+    <t>0.85 (N = 178)</t>
   </si>
   <si>
     <t>0.351 (N = 178)</t>
@@ -236,7 +299,7 @@
     <t>0.458 (N = 178)</t>
   </si>
   <si>
-    <t>0.325 (N = 178)</t>
+    <t>0.434 (N = 148)</t>
   </si>
   <si>
     <t>0.235 (N = 148)</t>
@@ -248,7 +311,19 @@
     <t>0.409 (N = 148)</t>
   </si>
   <si>
-    <t>0.517 (N = 148)</t>
+    <t>0.603 (N = 118)</t>
+  </si>
+  <si>
+    <t>0.454 (N = 118)</t>
+  </si>
+  <si>
+    <t>0.352 (N = 118)</t>
+  </si>
+  <si>
+    <t>0.265 (N = 118)</t>
+  </si>
+  <si>
+    <t>0.05 (N = 1092)</t>
   </si>
   <si>
     <t>0.009 (N = 1092)</t>
@@ -260,7 +335,7 @@
     <t>0.019 (N = 1092)</t>
   </si>
   <si>
-    <t>0.01 (N = 1092)</t>
+    <t>0.331 (N = 932)</t>
   </si>
   <si>
     <t>0.07 (N = 932)</t>
@@ -272,7 +347,7 @@
     <t>0.041 (N = 932)</t>
   </si>
   <si>
-    <t>0.001 (N = 932)</t>
+    <t>0.32 (N = 772)</t>
   </si>
   <si>
     <t>0.191 (N = 772)</t>
@@ -284,7 +359,19 @@
     <t>0.016 (N = 772)</t>
   </si>
   <si>
-    <t>0.013 (N = 772)</t>
+    <t>0.513 (N = 612)</t>
+  </si>
+  <si>
+    <t>0.146 (N = 612)</t>
+  </si>
+  <si>
+    <t>0.121 (N = 612)</t>
+  </si>
+  <si>
+    <t>0.02 (N = 612)</t>
+  </si>
+  <si>
+    <t>Frac. Difícil ELO p3 c3</t>
   </si>
   <si>
     <t>Frac. Difícil ELO p4 c3</t>
@@ -296,7 +383,7 @@
     <t>Frac. Difícil ELO p6 c3</t>
   </si>
   <si>
-    <t>Frac. Difícil ELO p7 c3</t>
+    <t>Frac. Difícil ELO p3 c4</t>
   </si>
   <si>
     <t>Frac. Difícil ELO p4 c4</t>
@@ -308,7 +395,7 @@
     <t>Frac. Difícil ELO p6 c4</t>
   </si>
   <si>
-    <t>Frac. Difícil ELO p7 c4</t>
+    <t>Frac. Difícil ELO p3 c5</t>
   </si>
   <si>
     <t>Frac. Difícil ELO p4 c5</t>
@@ -320,7 +407,19 @@
     <t>Frac. Difícil ELO p6 c5</t>
   </si>
   <si>
-    <t>Frac. Difícil ELO p7 c5</t>
+    <t>Frac. Difícil ELO p3 c6</t>
+  </si>
+  <si>
+    <t>Frac. Difícil ELO p4 c6</t>
+  </si>
+  <si>
+    <t>Frac. Difícil ELO p5 c6</t>
+  </si>
+  <si>
+    <t>Frac. Difícil ELO p6 c6</t>
+  </si>
+  <si>
+    <t>0.996 (N = 180)</t>
   </si>
   <si>
     <t>0.998 (N = 180)</t>
@@ -332,7 +431,7 @@
     <t>0.806 (N = 180)</t>
   </si>
   <si>
-    <t>0.724 (N = 180)</t>
+    <t>0.166 (N = 150)</t>
   </si>
   <si>
     <t>0.757 (N = 150)</t>
@@ -344,7 +443,7 @@
     <t>0.408 (N = 150)</t>
   </si>
   <si>
-    <t>0.186 (N = 150)</t>
+    <t>0.057 (N = 120)</t>
   </si>
   <si>
     <t>0.403 (N = 120)</t>
@@ -356,7 +455,19 @@
     <t>0.379 (N = 120)</t>
   </si>
   <si>
-    <t>0.161 (N = 120)</t>
+    <t>0.127 (N = 90)</t>
+  </si>
+  <si>
+    <t>0.467 (N = 90)</t>
+  </si>
+  <si>
+    <t>0.456 (N = 90)</t>
+  </si>
+  <si>
+    <t>0.695 (N = 90)</t>
+  </si>
+  <si>
+    <t>0.31 (N = 210)</t>
   </si>
   <si>
     <t>0.207 (N = 210)</t>
@@ -368,7 +479,7 @@
     <t>0.252 (N = 210)</t>
   </si>
   <si>
-    <t>0.143 (N = 210)</t>
+    <t>0.206 (N = 180)</t>
   </si>
   <si>
     <t>0.023 (N = 180)</t>
@@ -380,7 +491,7 @@
     <t>0.068 (N = 180)</t>
   </si>
   <si>
-    <t>0.044 (N = 180)</t>
+    <t>0.117 (N = 150)</t>
   </si>
   <si>
     <t>0.004 (N = 150)</t>
@@ -392,7 +503,19 @@
     <t>0.12 (N = 150)</t>
   </si>
   <si>
-    <t>0.054 (N = 150)</t>
+    <t>0.276 (N = 120)</t>
+  </si>
+  <si>
+    <t>0.008 (N = 120)</t>
+  </si>
+  <si>
+    <t>0.01 (N = 120)</t>
+  </si>
+  <si>
+    <t>0.023 (N = 120)</t>
+  </si>
+  <si>
+    <t>0.633 (N = 140)</t>
   </si>
   <si>
     <t>0.472 (N = 140)</t>
@@ -404,7 +527,7 @@
     <t>0.379 (N = 140)</t>
   </si>
   <si>
-    <t>0.502 (N = 140)</t>
+    <t>0.051 (N = 120)</t>
   </si>
   <si>
     <t>0.015 (N = 120)</t>
@@ -416,7 +539,7 @@
     <t>0.082 (N = 120)</t>
   </si>
   <si>
-    <t>0.32 (N = 120)</t>
+    <t>0.273 (N = 100)</t>
   </si>
   <si>
     <t>0.289 (N = 100)</t>
@@ -428,7 +551,19 @@
     <t>0.463 (N = 100)</t>
   </si>
   <si>
-    <t>0.291 (N = 100)</t>
+    <t>0.554 (N = 80)</t>
+  </si>
+  <si>
+    <t>0.725 (N = 80)</t>
+  </si>
+  <si>
+    <t>0.942 (N = 80)</t>
+  </si>
+  <si>
+    <t>0.964 (N = 80)</t>
+  </si>
+  <si>
+    <t>0.526 (N = 354)</t>
   </si>
   <si>
     <t>0.926 (N = 354)</t>
@@ -440,7 +575,7 @@
     <t>0.74 (N = 354)</t>
   </si>
   <si>
-    <t>0.572 (N = 354)</t>
+    <t>0.894 (N = 304)</t>
   </si>
   <si>
     <t>0.991 (N = 304)</t>
@@ -452,7 +587,7 @@
     <t>0.715 (N = 304)</t>
   </si>
   <si>
-    <t>0.855 (N = 304)</t>
+    <t>0.576 (N = 254)</t>
   </si>
   <si>
     <t>0.633 (N = 254)</t>
@@ -464,7 +599,19 @@
     <t>0.609 (N = 254)</t>
   </si>
   <si>
-    <t>0.686 (N = 254)</t>
+    <t>0.347 (N = 204)</t>
+  </si>
+  <si>
+    <t>0.486 (N = 204)</t>
+  </si>
+  <si>
+    <t>0.683 (N = 204)</t>
+  </si>
+  <si>
+    <t>0.185 (N = 204)</t>
+  </si>
+  <si>
+    <t>0.615 (N = 208)</t>
   </si>
   <si>
     <t>0.159 (N = 208)</t>
@@ -476,7 +623,7 @@
     <t>0.34 (N = 208)</t>
   </si>
   <si>
-    <t>0.564 (N = 208)</t>
+    <t>0.74 (N = 178)</t>
   </si>
   <si>
     <t>0.215 (N = 178)</t>
@@ -488,7 +635,7 @@
     <t>0.419 (N = 178)</t>
   </si>
   <si>
-    <t>0.697 (N = 178)</t>
+    <t>0.631 (N = 148)</t>
   </si>
   <si>
     <t>0.166 (N = 148)</t>
@@ -500,7 +647,19 @@
     <t>0.074 (N = 148)</t>
   </si>
   <si>
-    <t>0.053 (N = 148)</t>
+    <t>0.375 (N = 118)</t>
+  </si>
+  <si>
+    <t>0.299 (N = 118)</t>
+  </si>
+  <si>
+    <t>0.227 (N = 118)</t>
+  </si>
+  <si>
+    <t>0.173 (N = 118)</t>
+  </si>
+  <si>
+    <t>0.863 (N = 1092)</t>
   </si>
   <si>
     <t>0.834 (N = 1092)</t>
@@ -512,7 +671,7 @@
     <t>0.537 (N = 1092)</t>
   </si>
   <si>
-    <t>0.445 (N = 1092)</t>
+    <t>0.444 (N = 932)</t>
   </si>
   <si>
     <t>0.352 (N = 932)</t>
@@ -524,7 +683,7 @@
     <t>0.182 (N = 932)</t>
   </si>
   <si>
-    <t>0.325 (N = 932)</t>
+    <t>0.249 (N = 772)</t>
   </si>
   <si>
     <t>0.071 (N = 772)</t>
@@ -536,7 +695,16 @@
     <t>0.206 (N = 772)</t>
   </si>
   <si>
-    <t>0.073 (N = 772)</t>
+    <t>0.284 (N = 612)</t>
+  </si>
+  <si>
+    <t>0.17 (N = 612)</t>
+  </si>
+  <si>
+    <t>0.242 (N = 612)</t>
+  </si>
+  <si>
+    <t>0.136 (N = 612)</t>
   </si>
 </sst>
 </file>
@@ -894,7 +1062,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -928,22 +1096,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -951,22 +1119,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -974,22 +1142,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -997,22 +1165,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1020,22 +1188,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1043,22 +1211,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1066,22 +1234,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1089,22 +1257,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1112,22 +1280,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1135,22 +1303,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="G11" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1158,22 +1326,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1181,22 +1349,114 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
         <v>53</v>
       </c>
-      <c r="E13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" t="s">
-        <v>89</v>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1466,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1237,278 +1497,370 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="F2" t="s">
-        <v>150</v>
+        <v>198</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="F3" t="s">
-        <v>151</v>
+        <v>199</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
       <c r="F4" t="s">
-        <v>152</v>
+        <v>200</v>
       </c>
       <c r="G4" t="s">
-        <v>164</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="F5" t="s">
-        <v>153</v>
+        <v>201</v>
       </c>
       <c r="G5" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="F6" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="G6" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>187</v>
       </c>
       <c r="F7" t="s">
-        <v>155</v>
+        <v>203</v>
       </c>
       <c r="G7" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
+        <v>188</v>
       </c>
       <c r="F8" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="G8" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="F9" t="s">
-        <v>157</v>
+        <v>205</v>
       </c>
       <c r="G9" t="s">
-        <v>169</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
       <c r="F10" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="G10" t="s">
-        <v>170</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>175</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="F11" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
       <c r="G11" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="E12" t="s">
-        <v>148</v>
+        <v>192</v>
       </c>
       <c r="F12" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="G12" t="s">
-        <v>172</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="E13" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" t="s">
+        <v>196</v>
+      </c>
+      <c r="F16" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
         <v>149</v>
       </c>
-      <c r="F13" t="s">
-        <v>161</v>
-      </c>
-      <c r="G13" t="s">
-        <v>173</v>
+      <c r="C17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17" t="s">
+        <v>197</v>
+      </c>
+      <c r="F17" t="s">
+        <v>213</v>
+      </c>
+      <c r="G17" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>